<commit_message>
maj données et packages
</commit_message>
<xml_diff>
--- a/Google Pixel 7.xlsx
+++ b/Google Pixel 7.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -1068,6 +1068,1086 @@
         <v>399.0</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="3">
+        <v>250.76</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="3">
+        <v>273.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="3">
+        <v>298.77</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="3">
+        <v>256.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="3">
+        <v>257.81</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="3">
+        <v>266.57</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="3">
+        <v>255.72</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="3">
+        <v>248.95</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="3">
+        <v>268.6</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="3">
+        <v>312.77</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="3">
+        <v>392.9</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="3">
+        <v>431.73</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" s="3">
+        <v>329.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" s="3">
+        <v>396.63</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" s="3">
+        <v>423.74</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="3">
+        <v>324.48</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="3">
+        <v>366.87</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2">
+        <v>45677.0</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="3">
+        <v>398.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="3">
+        <v>256.98</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="3">
+        <v>267.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="3">
+        <v>290.3</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="3">
+        <v>256.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="3">
+        <v>257.81</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="3">
+        <v>263.57</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" s="3">
+        <v>255.72</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" s="3">
+        <v>250.56</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" s="3">
+        <v>264.61</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="3">
+        <v>290.36</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="3">
+        <v>383.15</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="3">
+        <v>414.1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F68" s="3">
+        <v>329.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F69" s="3">
+        <v>389.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F70" s="3">
+        <v>423.74</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F71" s="3">
+        <v>349.77</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F72" s="3">
+        <v>366.87</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2">
+        <v>45678.0</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" s="3">
+        <v>398.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" s="3">
+        <v>253.98</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" s="3">
+        <v>260.74</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" s="3">
+        <v>302.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F77" s="3">
+        <v>252.93</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F78" s="3">
+        <v>255.65</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79" s="3">
+        <v>262.14</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F80" s="3">
+        <v>255.72</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F81" s="3">
+        <v>248.76</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82" s="3">
+        <v>263.43</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" s="3">
+        <v>323.0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="3">
+        <v>385.7</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" s="3">
+        <v>400.13</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F86" s="3">
+        <v>334.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F87" s="3">
+        <v>379.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F88" s="3">
+        <v>385.7</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F89" s="3">
+        <v>349.77</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F90" s="3">
+        <v>368.79</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2">
+        <v>45679.0</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F91" s="3">
+        <v>398.0</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>